<commit_message>
model streamlining, added raw TB spawn data
</commit_message>
<xml_diff>
--- a/data/model-structural-parameters.xlsx
+++ b/data/model-structural-parameters.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-DegreeDay-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B783FC36-FD1C-FB4B-956E-82C0EB11128A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87BCFC6-D80D-2649-BB9D-297B964EF369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57620" yWindow="6860" windowWidth="14380" windowHeight="21100" xr2:uid="{B25F5835-D63E-524D-A408-87034025025D}"/>
+    <workbookView xWindow="17360" yWindow="500" windowWidth="16240" windowHeight="19220" xr2:uid="{B25F5835-D63E-524D-A408-87034025025D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="coefs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Colby &amp; Brooke (1973)</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -54,12 +51,6 @@
     <t>Stewart et al. (2021)</t>
   </si>
   <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Lake</t>
-  </si>
-  <si>
     <t>Pickeral Lake</t>
   </si>
   <si>
@@ -93,22 +84,37 @@
     <t>Lake Constance</t>
   </si>
   <si>
+    <t>Lake Geneva</t>
+  </si>
+  <si>
+    <t>Lake Bourget</t>
+  </si>
+  <si>
+    <t>morph</t>
+  </si>
+  <si>
+    <t>pelagic</t>
+  </si>
+  <si>
+    <t>littoral</t>
+  </si>
+  <si>
+    <t>unpublished Thonon</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>lake</t>
+  </si>
+  <si>
     <t>lavaretus ﻿wartmanni</t>
   </si>
   <si>
     <t>lavaretus ﻿macrophthalmus</t>
-  </si>
-  <si>
-    <t>Lake Geneva</t>
-  </si>
-  <si>
-    <t>Lake Bourget</t>
-  </si>
-  <si>
-    <t>lavaretus pelagic</t>
-  </si>
-  <si>
-    <t>lavaretus littoral</t>
   </si>
 </sst>
 </file>
@@ -464,235 +470,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D1BDFD-8A89-894E-97BB-528E9C5B8321}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-2.4087999999999998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-2.3576880999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.5691300000000003E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-3.2840000000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-2.399</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.238E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-2.0869999999999998E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-2.4275519999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4.4464999999999998E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.7919999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-2.404261</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.0426000000000002E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2.65E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-2.4087999999999998</v>
-      </c>
-      <c r="E2" s="1">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-2.3576880999999998</v>
-      </c>
-      <c r="E3" s="1">
-        <v>7.5691300000000003E-2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>-3.2840000000000001E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
-        <v>-2.399</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7.238E-2</v>
-      </c>
-      <c r="F4" s="1">
-        <v>-2.0869999999999998E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-2.3034949999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.5057000000000004E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4.3399999999999998E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-2.2418450000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.11035399999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-3.2694849999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-2.3001619999999998</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.11035399999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-3.0944890000000002E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1">
-        <v>-2.4256589000000002</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4.3399300000000002E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3.9172E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-2.1842999999999999</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.1199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
-        <v>-2.404261</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3.0426000000000002E-2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.65E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E11" s="1">
+        <v>-2.25169</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6.8690000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-2.0795499999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.8460000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1">
-        <v>-2.3034949999999998</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6.5057000000000004E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>4.3399999999999998E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-2.2418450000000001</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.11035399999999999</v>
-      </c>
-      <c r="F8" s="1">
-        <v>-3.2694849999999999E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-2.3001619999999998</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.11035399999999999</v>
-      </c>
-      <c r="F9" s="1">
-        <v>-3.0944890000000002E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>-2.1497099999999998</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>5.7360000000000001E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to moving averages
</commit_message>
<xml_diff>
--- a/data/model-structural-parameters.xlsx
+++ b/data/model-structural-parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B960BD7-0FBC-5146-A95C-954C02B14748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627A9A9A-73FA-CF4D-8BDF-8EA8A1CE0A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="500" windowWidth="27060" windowHeight="19220" xr2:uid="{B25F5835-D63E-524D-A408-87034025025D}"/>
+    <workbookView xWindow="13020" yWindow="500" windowWidth="20580" windowHeight="19220" xr2:uid="{B25F5835-D63E-524D-A408-87034025025D}"/>
   </bookViews>
   <sheets>
     <sheet name="coefficients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Colby &amp; Brooke (1973)</t>
   </si>
@@ -121,20 +121,6 @@
   </si>
   <si>
     <t>e</t>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -144,19 +130,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -499,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D1BDFD-8A89-894E-97BB-528E9C5B8321}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +497,7 @@
     <col min="8" max="8" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -542,11 +522,8 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -569,7 +546,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -583,19 +560,16 @@
         <v>6</v>
       </c>
       <c r="F3" s="1">
-        <v>-2.3576880999999998</v>
+        <v>-2.3289428999999999</v>
       </c>
       <c r="G3" s="1">
-        <v>7.5691300000000003E-2</v>
+        <v>7.1687699999999993E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>-3.2840000000000001E-4</v>
-      </c>
-      <c r="I3">
-        <v>0.99939999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-9.1399999999999999E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -609,19 +583,16 @@
         <v>7</v>
       </c>
       <c r="F4" s="1">
-        <v>-2.399</v>
+        <v>-2.3835484999999998</v>
       </c>
       <c r="G4" s="1">
-        <v>7.238E-2</v>
+        <v>6.4286399999999994E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>-2.0869999999999998E-5</v>
-      </c>
-      <c r="I4">
-        <v>0.99990000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8.4340000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -635,19 +606,16 @@
         <v>8</v>
       </c>
       <c r="F5" s="1">
-        <v>-2.4275519999999999</v>
+        <v>-2.4182630000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>4.4464999999999998E-2</v>
+        <v>4.5934000000000003E-2</v>
       </c>
       <c r="H5" s="1">
-        <v>3.7919999999999998E-3</v>
-      </c>
-      <c r="I5">
-        <v>0.99960000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.2160000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -661,19 +629,16 @@
         <v>8</v>
       </c>
       <c r="F6" s="1">
-        <v>-2.404261</v>
+        <v>-2.3663720000000001</v>
       </c>
       <c r="G6" s="1">
-        <v>3.0426000000000002E-2</v>
+        <v>8.8319999999999996E-3</v>
       </c>
       <c r="H6" s="1">
-        <v>2.65E-3</v>
-      </c>
-      <c r="I6">
-        <v>0.99850000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.0090000000000004E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -696,7 +661,7 @@
         <v>4.3399999999999998E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -722,7 +687,7 @@
         <v>-3.2694849999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -748,7 +713,7 @@
         <v>-3.0944890000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -765,16 +730,13 @@
         <v>15</v>
       </c>
       <c r="F10" s="1">
-        <v>-2.1842999999999999</v>
+        <v>-2.1347230000000001</v>
       </c>
       <c r="G10" s="1">
-        <v>6.1199999999999997E-2</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.5157999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -791,16 +753,13 @@
         <v>15</v>
       </c>
       <c r="F11" s="1">
-        <v>-2.25169</v>
+        <v>-2.1164149999999999</v>
       </c>
       <c r="G11" s="1">
-        <v>6.8690000000000001E-2</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.2711000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -814,16 +773,13 @@
         <v>17</v>
       </c>
       <c r="F12" s="1">
-        <v>-2.0795499999999998</v>
+        <v>-2.0688599999999999</v>
       </c>
       <c r="G12" s="1">
-        <v>4.8460000000000003E-2</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.7426999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -837,13 +793,10 @@
         <v>16</v>
       </c>
       <c r="F13" s="1">
-        <v>-2.1497099999999998</v>
+        <v>-2.1159439999999998</v>
       </c>
       <c r="G13" s="1">
-        <v>5.7360000000000001E-2</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
+        <v>5.2842E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>